<commit_message>
Add FMD scenario for cattle. Update disease impacts and re-run SR.
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/Disease specific attribution/scenarios/sr_disease_scenarios.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/Disease specific attribution/scenarios/sr_disease_scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alarkins/Desktop/Disease specific attribution/scenarios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alarkins/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/Disease specific attribution/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA50DD5-DCCD-0F49-9F0A-83863E2D879F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2D4E5A-0326-CA43-8620-26DF56AF31B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-620" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="368">
   <si>
     <t>AHLE Parameter</t>
   </si>
@@ -289,16 +289,16 @@
     <t>0.44</t>
   </si>
   <si>
-    <t>rpert(10000,0.528155141733642,0.52973352286904,0.529221898639954)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.438519598041629,0.439825022490247,0.439383807379672)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.529946122168983,0.529996022114311,0.529988775605057)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.439954122705182,0.439996821575658,0.439992084259372)</t>
+    <t>rpert(10000,0.523923412028754,0.529115820613565,0.527810438094783)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.435883731955272,0.439453108573222,0.438348233232671)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.529945212758172,0.529997020922543,0.529988805770719)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.439959556904763,0.439997254835068,0.43999065937699)</t>
   </si>
   <si>
     <t>milk_value_ltr</t>
@@ -373,28 +373,28 @@
     <t>rpert(1000, 0.03/6, 0.6/6, 0.18/6)</t>
   </si>
   <si>
-    <t>rpert(10000,0.000134409553486073,0.00318257611850059,0.00069330785023264)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000125497506048066,0.00341333137765322,0.000745766802664381)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000219213890368434,0.00593630288691467,0.00152689410919792)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000224633890833908,0.00627277757241471,0.00157102219195532)</t>
-  </si>
-  <si>
-    <t>rpert(10000,4.3628505189944e-06,9.11286955384516e-05,1.12943636433325e-05)</t>
-  </si>
-  <si>
-    <t>rpert(10000,5.2930885457337e-06,0.00010469102317625,9.9881149428775e-06)</t>
-  </si>
-  <si>
-    <t>rpert(10000,8.62087594136897e-06,0.000125344922087001,1.72414524797603e-05)</t>
-  </si>
-  <si>
-    <t>rpert(10000,9.55742238943119e-06,0.000109378340449445,2.31003615870557e-05)</t>
+    <t>rpert(10000,0.000116991131170659,0.00308182299443404,0.00072391355732723)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000127187746603674,0.00366798992416746,0.000686781599267169)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000218074714808748,0.00604780861825356,0.00151895764218581)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000192606574424708,0.00621909822636434,0.00160852052989736)</t>
+  </si>
+  <si>
+    <t>rpert(10000,4.98699322214014e-06,7.44407807978191e-05,1.53647531196854e-05)</t>
+  </si>
+  <si>
+    <t>rpert(10000,6.82697330647405e-06,7.6736266251838e-05,1.65279681172381e-05)</t>
+  </si>
+  <si>
+    <t>rpert(10000,8.79191355919839e-06,9.81199805677948e-05,2.41897075908163e-05)</t>
+  </si>
+  <si>
+    <t>rpert(10000,8.32651329783294e-06,0.000122008634736724,2.04025417814401e-05)</t>
   </si>
   <si>
     <t>AlphaJ</t>
@@ -409,16 +409,16 @@
     <t>rpert(1000, 0.14/6, 0.14/6, 0.14/6)</t>
   </si>
   <si>
-    <t>rpert(10000,0.000156285330324334,0.00367832646265846,0.000743208813731075)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000179586502752257,0.00367252014395997,0.000867899725084099)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000231474046099103,0.00581060841268544,0.00161366020291672)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000239006549759046,0.00672958170746777,0.00153040606991434)</t>
+    <t>rpert(10000,0.000141031310519345,0.00340220135410079,0.00083399372363374)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000162844448936618,0.00398207246568165,0.000795786779628026)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000215060351037448,0.00618790970533828,0.00153052368058862)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.00018013042288901,0.00614275060912874,0.00168356687637067)</t>
   </si>
   <si>
     <t>AlphaF</t>
@@ -433,28 +433,28 @@
     <t>rpert(1000, 0.04/12, 0.13/12, 0.09/12)</t>
   </si>
   <si>
-    <t>rpert(10000,0.000111203699374363,0.00225612635379497,0.000474930308149419)</t>
-  </si>
-  <si>
-    <t>rpert(10000,9.81092658411735e-05,0.00202848955376356,0.000400598027654353)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000178062258548949,0.00405904404514038,0.000885796921723272)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000149298359997603,0.00381912876797322,0.000856268343858346)</t>
-  </si>
-  <si>
-    <t>rpert(10000,2.79265990081844e-07,6.22972404900476e-06,4.59501657389016e-07)</t>
-  </si>
-  <si>
-    <t>rpert(10000,2.33251758310198e-07,4.28564751655911e-06,6.94173005178241e-07)</t>
-  </si>
-  <si>
-    <t>rpert(10000,3.74758207148485e-07,8.08014910499898e-06,6.48996249892217e-07)</t>
-  </si>
-  <si>
-    <t>rpert(10000,3.02235466635892e-07,6.87894445593757e-06,8.28058406200538e-07)</t>
+    <t>rpert(10000,0.000101707205400686,0.00199125154523217,0.000549392593271463)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.00010049374683891,0.00187709206837283,0.000432966896295771)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000153730524337801,0.00383200154754454,0.000949210723727086)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000131739628682422,0.00345962128787474,0.00094508788788562)</t>
+  </si>
+  <si>
+    <t>rpert(10000,2.99342057431439e-07,5.19176405038013e-06,7.08762193691861e-07)</t>
+  </si>
+  <si>
+    <t>rpert(10000,2.5458489470098e-07,4.0529780163037e-06,7.4770053146625e-07)</t>
+  </si>
+  <si>
+    <t>rpert(10000,4.34484040413051e-07,5.75594065731715e-06,1.22615481721307e-06)</t>
+  </si>
+  <si>
+    <t>rpert(10000,3.53115412858233e-07,6.14542146517148e-06,9.98021812525498e-07)</t>
   </si>
   <si>
     <t>AlphaM</t>
@@ -469,16 +469,16 @@
     <t>rpert(1000, 0.05/12, 0.13/12, 0.09/12)</t>
   </si>
   <si>
-    <t>rpert(10000,4.63892260651343e-05,0.000887594013659135,0.000210123276857232)</t>
-  </si>
-  <si>
-    <t>rpert(10000,5.99688198971096e-05,0.00144855363983377,0.000320917989880937)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000106290730544208,0.00218450566573271,0.000541921974355401)</t>
-  </si>
-  <si>
-    <t>rpert(10000,9.00786247422695e-05,0.00239539756314924,0.000656004581743383)</t>
+    <t>rpert(10000,5.32181839037925e-05,0.000827688430141543,0.000221916072060784)</t>
+  </si>
+  <si>
+    <t>rpert(10000,7.45204866079051e-05,0.00138907157158103,0.000328004453334497)</t>
+  </si>
+  <si>
+    <t>rpert(10000,7.35086724051142e-05,0.00222836053782904,0.000541253137663935)</t>
+  </si>
+  <si>
+    <t>rpert(10000,8.33011922070789e-05,0.00238080653962697,0.000659368795289837)</t>
   </si>
   <si>
     <t># Culls</t>
@@ -1018,6 +1018,30 @@
     <t>rpert(10000, (260/12), (649/12), (368/12))</t>
   </si>
   <si>
+    <t>rpert(10000,21.5460302592659,52.6417849892953,30.5741431427786)</t>
+  </si>
+  <si>
+    <t>rpert(10000,21.5184620246659,52.6576510448321,30.6627727865869)</t>
+  </si>
+  <si>
+    <t>rpert(10000,21.3501908638026,51.707692784256,30.8527773878429)</t>
+  </si>
+  <si>
+    <t>rpert(10000,21.5242344108972,51.5260766881842,30.8185135489957)</t>
+  </si>
+  <si>
+    <t>rpert(10000,21.7450206711001,51.8163363211342,31.2165280347598)</t>
+  </si>
+  <si>
+    <t>rpert(10000,21.8295844987448,52.9607800751334,30.8135508337074)</t>
+  </si>
+  <si>
+    <t>rpert(10000,21.898112415062,52.0216696706451,31.1463660426073)</t>
+  </si>
+  <si>
+    <t>rpert(10000,21.8118158642296,51.3334544864124,31.2930014051047)</t>
+  </si>
+  <si>
     <t>lab_non_health</t>
   </si>
   <si>
@@ -1042,28 +1066,22 @@
     <t>runif(10000, (2.2/12), (2.8/12))</t>
   </si>
   <si>
-    <t>rpert(10000,0.0205278646084586,0.227378754837726,0.0618594104675901)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.0211540354228057,0.234592558320033,0.0672248656376064)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.0213833239642956,0.225218583671154,0.0923550993556093)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.0204636747401951,0.257664760909479,0.0908553582092941)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000953414566923747,0.0149432775181118,0.00282777078498726)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000989380592422069,0.0158960961185475,0.00300169902817774)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.00122892092924821,0.0211569136728329,0.00422124853153377)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.00151380758490779,0.0248628593215218,0.00363265746359942)</t>
+    <t>rpert(10000,0.000453471880004924,0.367585542549371,0.0108778126416506)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000463058949761048,0.331669957628834,0.0262369517356783)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000711930430477487,0.368885907931813,0.0365735213317957)</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.00135390733998949,0.47014876961416,0.0154219670177168)</t>
+  </si>
+  <si>
+    <t>rpert(10000,7.23688976228906e-05,0.0229744086777663,0.000294599142606751)</t>
+  </si>
+  <si>
+    <t>rpert(10000,3.28357529476166e-05,0.0317286983442613,0.000444535321097627)</t>
   </si>
   <si>
     <t>## Capital costs</t>
@@ -1076,67 +1094,6 @@
   </si>
   <si>
     <t>Infrastructure_per_head</t>
-  </si>
-  <si>
-    <r>
-      <t>rpert(10000,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>.52</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,1.68664153251267,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1158,7 +1115,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,1.70937960173152,</t>
+      <t>,1.68776885423172,</t>
     </r>
     <r>
       <rPr>
@@ -1189,6 +1146,47 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
+      <t>0.52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,1.68444392828578,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>0.8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rpert(10000,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
       <t>0.37</t>
     </r>
     <r>
@@ -1199,7 +1197,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,1.18747584839876,</t>
+      <t>,1.1821387779818,0.84585973838507)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>rpert(10000,0.386868919190795,1.19023714895814,</t>
     </r>
     <r>
       <rPr>
@@ -1230,7 +1233,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>0.37</t>
+      <t>0.52</t>
     </r>
     <r>
       <rPr>
@@ -1240,7 +1243,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,1.19421042763217,0.842839370520885)</t>
+      <t>,1.10081194389654,0.797872454592452)</t>
     </r>
   </si>
   <si>
@@ -1263,7 +1266,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,1.1062155419979,</t>
+      <t>,1.11119335266897,</t>
     </r>
     <r>
       <rPr>
@@ -1294,7 +1297,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>0.52</t>
+      <t>0.55</t>
     </r>
     <r>
       <rPr>
@@ -1304,7 +1307,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,1.11283129614805,</t>
+      <t>,1.11019063553329,</t>
     </r>
     <r>
       <rPr>
@@ -1312,7 +1315,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>0.80</t>
+      <t>0.85</t>
     </r>
     <r>
       <rPr>
@@ -1345,30 +1348,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,1.10875652753617,0.849409699349612)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>rpert(10000,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>0.55</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,1.11370816870116,</t>
+      <t>,1.10762138066658,</t>
     </r>
     <r>
       <rPr>
@@ -1389,12 +1369,18 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>rpert(10000,0.0000439356969377126,0.0271374707216779,0.00115275781364292)</t>
+  </si>
+  <si>
+    <t>rpert(10000,3.4050810942168e-05,0.032612289922902,2.00186154478751e-05)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1414,13 +1400,6 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1754,16 +1733,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O115" sqref="O115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="3" max="6" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="72.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="71.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="70.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="71.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="71.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="70.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="71.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2311,28 +2300,28 @@
         <v>67</v>
       </c>
       <c r="K15" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="L15" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="M15" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="N15" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="O15" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="P15" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="Q15" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="R15" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -4921,45 +4910,45 @@
         <v>331</v>
       </c>
       <c r="K108" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="L108" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="M108" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="N108" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="O108" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="P108" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="Q108" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="R108" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="C109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="D109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="E109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="F109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="G109" t="s">
         <v>277</v>
@@ -4974,33 +4963,33 @@
         <v>277</v>
       </c>
       <c r="K109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="L109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="M109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="N109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="O109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="P109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="Q109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="R109" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.2">
@@ -5010,20 +4999,20 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="B115" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="C115" t="s">
         <v>79</v>
@@ -5038,55 +5027,55 @@
         <v>79</v>
       </c>
       <c r="G115" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="H115" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="I115" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="J115" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="K115" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="L115" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="M115" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="N115" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="O115" t="s">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="P115" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="Q115" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="R115" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="C119" t="s">
         <v>79</v>
@@ -5139,7 +5128,7 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C120" t="s">
         <v>277</v>

</xml_diff>

<commit_message>
Rerun SR scenarios with updated parameters and impact duration
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/Disease specific attribution/scenarios/sr_disease_scenarios.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/Disease specific attribution/scenarios/sr_disease_scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alarkins/Documents/GitHub/GBADsLiverpool/Ethiopia Workspace/Code and Control Files/Disease specific attribution/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2D4E5A-0326-CA43-8620-26DF56AF31B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7856FF-B22C-1F4F-A576-BB8E720E0FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-620" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="364">
   <si>
     <t>AHLE Parameter</t>
   </si>
@@ -1064,24 +1064,6 @@
   </si>
   <si>
     <t>runif(10000, (2.2/12), (2.8/12))</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000453471880004924,0.367585542549371,0.0108778126416506)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000463058949761048,0.331669957628834,0.0262369517356783)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.000711930430477487,0.368885907931813,0.0365735213317957)</t>
-  </si>
-  <si>
-    <t>rpert(10000,0.00135390733998949,0.47014876961416,0.0154219670177168)</t>
-  </si>
-  <si>
-    <t>rpert(10000,7.23688976228906e-05,0.0229744086777663,0.000294599142606751)</t>
-  </si>
-  <si>
-    <t>rpert(10000,3.28357529476166e-05,0.0317286983442613,0.000444535321097627)</t>
   </si>
   <si>
     <t>## Capital costs</t>
@@ -1202,29 +1184,6 @@
   </si>
   <si>
     <r>
-      <t>rpert(10000,0.386868919190795,1.19023714895814,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>0.85</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>rpert(10000,</t>
     </r>
     <r>
@@ -1370,10 +1329,57 @@
     </r>
   </si>
   <si>
-    <t>rpert(10000,0.0000439356969377126,0.0271374707216779,0.00115275781364292)</t>
-  </si>
-  <si>
-    <t>rpert(10000,3.4050810942168e-05,0.032612289922902,2.00186154478751e-05)</t>
+    <t>rpert(10000,0.000453471880004924*1000,0.367585542549371*1000,0.0108778126416506*1000)/1000</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000463058949761048*1000,0.331669957628834*1000,0.0262369517356783*1000)/1000</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.000711930430477487*1000,0.368885907931813*1000,0.0365735213317957*1000)/1000</t>
+  </si>
+  <si>
+    <t>rpert(10000,0.00135390733998949*1000,0.47014876961416*1000,0.0154219670177168*1000)/1000</t>
+  </si>
+  <si>
+    <r>
+      <t>rpert(10000,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>0.37</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,1.19023714895814,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>0.85</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1733,9 +1739,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O115" sqref="O115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2300,28 +2306,28 @@
         <v>67</v>
       </c>
       <c r="K15" t="s">
+        <v>352</v>
+      </c>
+      <c r="L15" t="s">
+        <v>355</v>
+      </c>
+      <c r="M15" t="s">
+        <v>354</v>
+      </c>
+      <c r="N15" t="s">
+        <v>357</v>
+      </c>
+      <c r="O15" t="s">
+        <v>353</v>
+      </c>
+      <c r="P15" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>363</v>
+      </c>
+      <c r="R15" t="s">
         <v>358</v>
-      </c>
-      <c r="L15" t="s">
-        <v>362</v>
-      </c>
-      <c r="M15" t="s">
-        <v>360</v>
-      </c>
-      <c r="N15" t="s">
-        <v>364</v>
-      </c>
-      <c r="O15" t="s">
-        <v>359</v>
-      </c>
-      <c r="P15" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>361</v>
-      </c>
-      <c r="R15" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -5039,43 +5045,43 @@
         <v>347</v>
       </c>
       <c r="K115" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="L115" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="M115" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="N115" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="O115" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="P115" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="Q115" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="R115" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C119" t="s">
         <v>79</v>
@@ -5128,7 +5134,7 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="C120" t="s">
         <v>277</v>

</xml_diff>